<commit_message>
Revalidando exercicios do Pandas
</commit_message>
<xml_diff>
--- a/Pandas/PlanilhaProjeto.xlsx
+++ b/Pandas/PlanilhaProjeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WINDOWS\Desktop\JS\Python-temporário\Pandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D626AA-1231-4D88-BB78-D69501A1791C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01600343-2DCC-4B90-9A3F-02CC9AA1E4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,8 +80,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,103 +363,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G4:J9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="B11" sqref="B11:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="I4" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="J4" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <f ca="1">TODAY()</f>
+        <v>44763</v>
+      </c>
+      <c r="B2">
         <f ca="1">RANDBETWEEN(0, 50)</f>
-        <v>47</v>
-      </c>
-      <c r="I5">
-        <f ca="1">J5*H5</f>
-        <v>329</v>
-      </c>
-      <c r="J5">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <f ca="1">D2*B2</f>
+        <v>675</v>
+      </c>
+      <c r="D2">
         <f ca="1">RANDBETWEEN(5, 46)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H6">
-        <f t="shared" ref="H6:H9" ca="1" si="0">RANDBETWEEN(0, 100)</f>
-        <v>33</v>
-      </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I9" ca="1" si="1">J6*H6</f>
-        <v>528</v>
-      </c>
-      <c r="J6">
-        <f t="shared" ref="J6:J9" ca="1" si="2">RANDBETWEEN(5, 46)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H7">
-        <f t="shared" ca="1" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="I7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f t="shared" ref="A3:A10" ca="1" si="0">TODAY()</f>
+        <v>44763</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B11" ca="1" si="1">RANDBETWEEN(0, 100)</f>
+        <v>88</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C6" ca="1" si="2">D3*B3</f>
+        <v>1936</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" ca="1" si="3">RANDBETWEEN(5, 46)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44763</v>
+      </c>
+      <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>2009</v>
-      </c>
-      <c r="J7">
+        <v>71</v>
+      </c>
+      <c r="C4">
         <f t="shared" ca="1" si="2"/>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H8">
-        <f t="shared" ca="1" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="I8">
+        <v>710</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44763</v>
+      </c>
+      <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>476</v>
-      </c>
-      <c r="J8">
+        <v>55</v>
+      </c>
+      <c r="C5">
         <f t="shared" ca="1" si="2"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H9">
-        <f t="shared" ca="1" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="I9">
+        <v>2530</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="3"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44763</v>
+      </c>
+      <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>630</v>
-      </c>
-      <c r="J9">
+        <v>52</v>
+      </c>
+      <c r="C6">
         <f t="shared" ca="1" si="2"/>
-        <v>45</v>
+        <v>1560</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="3"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44763</v>
+      </c>
+      <c r="B7">
+        <f ca="1">RANDBETWEEN(0, 50)</f>
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <f ca="1">D7*B7</f>
+        <v>696</v>
+      </c>
+      <c r="D7">
+        <f ca="1">RANDBETWEEN(5, 46)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44763</v>
+      </c>
+      <c r="B8">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:C11" ca="1" si="4">D8*B8</f>
+        <v>2418</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="3"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44763</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ca="1" si="1"/>
+        <v>55</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="4"/>
+        <v>990</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" ca="1" si="0"/>
+        <v>44763</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="3"/>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>